<commit_message>
updated query5 to include data import and larger solve
</commit_message>
<xml_diff>
--- a/assignment_data_5.xlsx
+++ b/assignment_data_5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\next-best-position\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C034233-CB12-4CF8-A97D-15763451FBA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63FB8C06-59F8-4437-84AD-01C0912D6A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1B66F183-0BCD-4F97-8FF8-4BD92C1308AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{1B66F183-0BCD-4F97-8FF8-4BD92C1308AE}"/>
   </bookViews>
   <sheets>
     <sheet name="matches" sheetId="4" r:id="rId1"/>
@@ -419,7 +419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3B8DB73-2F44-4CE4-8C25-DBC453EF110E}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -2410,8 +2410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{359C2FAD-099F-46C8-A0D9-E07FF297F409}">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="A1:D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>